<commit_message>
final push app trader
</commit_message>
<xml_diff>
--- a/halloween_apps.xlsx
+++ b/halloween_apps.xlsx
@@ -1,26 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wteuc\Desktop\NSS\SQL\Projects\app_trader-kitkat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{AE0F8D2A-565C-488E-8980-E1CAAAC05EC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56915DD1-4EE0-465E-9499-77677EDD90AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4815" yWindow="525" windowWidth="21855" windowHeight="14925"/>
+    <workbookView xWindow="8235" yWindow="165" windowWidth="19320" windowHeight="15180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="combined_halloween" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
+    <sheet name="combined_halloween" sheetId="1" r:id="rId2"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId3"/>
+    <externalReference r:id="rId4"/>
+  </externalReferences>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="49">
   <si>
     <t>name</t>
   </si>
@@ -150,11 +155,29 @@
   <si>
     <t xml:space="preserve">Top 5 Halloween Recommendations </t>
   </si>
+  <si>
+    <t>games</t>
+  </si>
+  <si>
+    <t>shopping</t>
+  </si>
+  <si>
+    <t>food &amp; drink</t>
+  </si>
+  <si>
+    <t>news</t>
+  </si>
+  <si>
+    <t>health &amp; fitness</t>
+  </si>
+  <si>
+    <t>Music</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
   </numFmts>
@@ -294,7 +317,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="40">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -474,6 +497,48 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF002060"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -635,13 +700,20 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="39" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -701,6 +773,1588 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>EXPECTED</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> PROFIT</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-CA1D-4768-A65C-736CCCE71126}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-CA1D-4768-A65C-736CCCE71126}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-CA1D-4768-A65C-736CCCE71126}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="C00000"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-CA1D-4768-A65C-736CCCE71126}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000009-CA1D-4768-A65C-736CCCE71126}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="5"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000B-CA1D-4768-A65C-736CCCE71126}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="6"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000D-CA1D-4768-A65C-736CCCE71126}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="7"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="bg2">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000F-CA1D-4768-A65C-736CCCE71126}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="8"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="00B0F0"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000011-CA1D-4768-A65C-736CCCE71126}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="9"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000013-CA1D-4768-A65C-736CCCE71126}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="10"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000015-CA1D-4768-A65C-736CCCE71126}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="11"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000017-CA1D-4768-A65C-736CCCE71126}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="12"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000019-CA1D-4768-A65C-736CCCE71126}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:cat>
+            <c:strRef>
+              <c:f>[1]top_10_profit!$A$2:$A$14</c:f>
+              <c:strCache>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>PewDiePie's Tuber Simulator</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Hitman Sniper</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Cytus</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>ASOS</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Domino's Pizza USA</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Egg, Inc.</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Geometry Dash Lite</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>The Guardian</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>H*nest Meditation</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Dude Perfect</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>App Store Average Profit(not common)</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Play Store Average Profit(not common)</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Common Apps Average Profit</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>[1]top_10_profit!$B$2:$B$14</c:f>
+              <c:numCache>
+                <c:formatCode>"$"#,##0.00_);[Red]\("$"#,##0.00\)</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>475000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>470200</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>465100</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>460000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>460000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>460000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>460000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>460000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>458200</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>457100</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>112537.84</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>131907.70000000001</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>396298.49</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000001A-CA1D-4768-A65C-736CCCE71126}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="2027020799"/>
+        <c:axId val="2027022047"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="2027020799"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2027022047"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2027022047"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2027020799"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Top</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> 5 Halloween App Recommendations</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>combined_halloween!$D$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>purchase_cost</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="7030A0"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>combined_halloween!$A$3:$A$7</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Zombie Catchers</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Plants vs. Zombies 2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Plants vs. Zombies Heroes</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Zombie Tsunami</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>HauntedPic</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>combined_halloween!$D$3:$D$7</c:f>
+              <c:numCache>
+                <c:formatCode>"$"#,##0.00_);[Red]\("$"#,##0.00\)</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9900</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-BC6D-4F2A-BE64-32DED90C9D22}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>combined_halloween!$E$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>combined_profit</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FFFF00"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000002-BC6D-4F2A-BE64-32DED90C9D22}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:cat>
+            <c:strRef>
+              <c:f>combined_halloween!$A$3:$A$7</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Zombie Catchers</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Plants vs. Zombies 2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Plants vs. Zombies Heroes</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Zombie Tsunami</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>HauntedPic</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>combined_halloween!$E$3:$E$7</c:f>
+              <c:numCache>
+                <c:formatCode>"$"#,##0.00_);[Red]\("$"#,##0.00\)</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>438000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>427000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>427000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>427000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>188100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-BC6D-4F2A-BE64-32DED90C9D22}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1124774095"/>
+        <c:axId val="1763740351"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1124774095"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1763740351"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1763740351"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1124774095"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Play</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Store Average Profit by Genre</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-DA19-4E31-AAD5-6CDDC02ED33C}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="00B0F0"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-DA19-4E31-AAD5-6CDDC02ED33C}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FFFF00"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000004-DA19-4E31-AAD5-6CDDC02ED33C}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="002060"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-DA19-4E31-AAD5-6CDDC02ED33C}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000002-DA19-4E31-AAD5-6CDDC02ED33C}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:cat>
+            <c:strRef>
+              <c:f>'[2]Play Store genre avg profit'!$A$1:$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Board</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Health &amp; Fitness</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Comics</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Music</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Puzzle</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'[2]Play Store genre avg profit'!$B$1:$B$5</c:f>
+              <c:numCache>
+                <c:formatCode>"$"#,##0.00_);[Red]\("$"#,##0.00\)</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>179100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>164000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>164000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>156700</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>155000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-DA19-4E31-AAD5-6CDDC02ED33C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1509930656"/>
+        <c:axId val="1509931072"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1509930656"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Genre</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1509931072"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1509931072"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Avg</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> Profit</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1509930656"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -1142,7 +2796,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -1607,7 +3261,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -2002,7 +3656,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -2614,6 +4268,126 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -4626,7 +6400,1710 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DB8DCBC7-A2A8-4B52-8A71-05492CC62554}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1B80D5F7-8147-4916-B3EE-26EA331D9EE3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>352425</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="TextBox 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4B76109D-EC06-F44C-AFA1-AABE9CC712C1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7667625" y="419100"/>
+          <a:ext cx="7419975" cy="1266825"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Our</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> recommendation for price range would be to purchase apps with 5 star ratings with a $0.99, and to purchase apps on both platforms. The expected price range will be ~$500,000. The top 10 most profitable apps are on the graph to the left. The most profitable genre is the game app genre. For Halloween, we focused on the zombie game app market, as they were the most profitable on each platform. There were only 4 games with top profits for both platforms, so we also recommend the most profitable Halloween themed app from the apple store, Haunted Pic. </a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>114299</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>85724</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="11" name="Chart 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D8A56A26-799F-418C-88DC-A9C640E25FB9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -4773,6 +8250,180 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="top_10_profit"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="2">
+          <cell r="A2" t="str">
+            <v>PewDiePie's Tuber Simulator</v>
+          </cell>
+          <cell r="B2">
+            <v>475000</v>
+          </cell>
+        </row>
+        <row r="3">
+          <cell r="A3" t="str">
+            <v>Hitman Sniper</v>
+          </cell>
+          <cell r="B3">
+            <v>470200</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="A4" t="str">
+            <v>Cytus</v>
+          </cell>
+          <cell r="B4">
+            <v>465100</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="A5" t="str">
+            <v>ASOS</v>
+          </cell>
+          <cell r="B5">
+            <v>460000</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="A6" t="str">
+            <v>Domino's Pizza USA</v>
+          </cell>
+          <cell r="B6">
+            <v>460000</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="A7" t="str">
+            <v>Egg, Inc.</v>
+          </cell>
+          <cell r="B7">
+            <v>460000</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="A8" t="str">
+            <v>Geometry Dash Lite</v>
+          </cell>
+          <cell r="B8">
+            <v>460000</v>
+          </cell>
+        </row>
+        <row r="9">
+          <cell r="A9" t="str">
+            <v>The Guardian</v>
+          </cell>
+          <cell r="B9">
+            <v>460000</v>
+          </cell>
+        </row>
+        <row r="10">
+          <cell r="A10" t="str">
+            <v>H*nest Meditation</v>
+          </cell>
+          <cell r="B10">
+            <v>458200</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="A11" t="str">
+            <v>Dude Perfect</v>
+          </cell>
+          <cell r="B11">
+            <v>457100</v>
+          </cell>
+        </row>
+        <row r="12">
+          <cell r="A12" t="str">
+            <v>App Store Average Profit(not common)</v>
+          </cell>
+          <cell r="B12">
+            <v>112537.84</v>
+          </cell>
+        </row>
+        <row r="13">
+          <cell r="A13" t="str">
+            <v>Play Store Average Profit(not common)</v>
+          </cell>
+          <cell r="B13">
+            <v>131907.70000000001</v>
+          </cell>
+        </row>
+        <row r="14">
+          <cell r="A14" t="str">
+            <v>Common Apps Average Profit</v>
+          </cell>
+          <cell r="B14">
+            <v>396298.49</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="App Store genre avg profit"/>
+      <sheetName val="Play Store genre avg profit"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1">
+        <row r="1">
+          <cell r="A1" t="str">
+            <v>Board</v>
+          </cell>
+          <cell r="B1">
+            <v>179100</v>
+          </cell>
+        </row>
+        <row r="2">
+          <cell r="A2" t="str">
+            <v>Health &amp; Fitness</v>
+          </cell>
+          <cell r="B2">
+            <v>164000</v>
+          </cell>
+        </row>
+        <row r="3">
+          <cell r="A3" t="str">
+            <v>Comics</v>
+          </cell>
+          <cell r="B3">
+            <v>164000</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="A4" t="str">
+            <v>Music</v>
+          </cell>
+          <cell r="B4">
+            <v>156700</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="A5" t="str">
+            <v>Puzzle</v>
+          </cell>
+          <cell r="B5">
+            <v>155000</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5071,10 +8722,71 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A25F9A64-7F07-474F-BFC2-47D5B8059922}">
+  <dimension ref="N12:O18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S17" sqref="S17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="15" max="15" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="12" spans="14:15" x14ac:dyDescent="0.25">
+      <c r="N12" s="4"/>
+      <c r="O12" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="13" spans="14:15" x14ac:dyDescent="0.25">
+      <c r="N13" s="5"/>
+      <c r="O13" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="14:15" x14ac:dyDescent="0.25">
+      <c r="N14" s="6"/>
+      <c r="O14" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="15" spans="14:15" x14ac:dyDescent="0.25">
+      <c r="N15" s="7"/>
+      <c r="O15" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="16" spans="14:15" x14ac:dyDescent="0.25">
+      <c r="N16" s="8"/>
+      <c r="O16" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="17" spans="14:15" x14ac:dyDescent="0.25">
+      <c r="N17" s="9"/>
+      <c r="O17" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="14:15" x14ac:dyDescent="0.25">
+      <c r="N18" s="10"/>
+      <c r="O18" t="s">
+        <v>48</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I66"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N15" sqref="N15"/>
     </sheetView>
   </sheetViews>
@@ -5600,26 +9312,26 @@
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A64" s="2" t="s">
+      <c r="A64" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B64" s="2"/>
-      <c r="C64" s="2"/>
-      <c r="D64" s="2"/>
-      <c r="E64" s="2"/>
-      <c r="F64" s="2"/>
-      <c r="G64" s="2"/>
+      <c r="B64" s="3"/>
+      <c r="C64" s="3"/>
+      <c r="D64" s="3"/>
+      <c r="E64" s="3"/>
+      <c r="F64" s="3"/>
+      <c r="G64" s="3"/>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A66" s="3" t="s">
+      <c r="A66" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B66" s="3"/>
-      <c r="C66" s="3"/>
-      <c r="D66" s="3"/>
-      <c r="E66" s="3"/>
-      <c r="F66" s="3"/>
-      <c r="G66" s="3"/>
+      <c r="B66" s="2"/>
+      <c r="C66" s="2"/>
+      <c r="D66" s="2"/>
+      <c r="E66" s="2"/>
+      <c r="F66" s="2"/>
+      <c r="G66" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>